<commit_message>
started new bacterial GO term nb
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/DN/TD+ND/DN80_combined_TD+ND_bp_GO.xlsx
+++ b/analyses/unipept/GO-terms/DN/TD+ND/DN80_combined_TD+ND_bp_GO.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DN80_combined_TD+ND_bp_GO" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="revigo" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="organizing" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="for python" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="over 2" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="1111">
   <si>
     <t xml:space="preserve">GO term</t>
   </si>
@@ -3549,11 +3550,11 @@
   </sheetPr>
   <dimension ref="A1:E382"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A340" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.78"/>
@@ -7739,14 +7740,14 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.6"/>
   </cols>
@@ -19002,14 +19003,14 @@
   <dimension ref="A1:J403"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A386" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C111" activeCellId="0" sqref="C111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.73"/>
@@ -29905,11 +29906,11 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="5" width="11.54"/>
@@ -30100,6 +30101,2878 @@
       </c>
       <c r="E11" s="5" t="n">
         <v>22.8144989339019</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E218"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.98"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E123" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E130" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D131" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D132" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E132" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D133" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D134" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E134" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E135" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D136" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E136" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D137" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E137" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E140" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D141" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E141" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E144" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E145" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E146" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E149" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E150" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E154" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E156" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D157" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E157" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D159" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E161" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E162" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E164" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E165" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D167" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E167" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D169" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E176" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E186" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E187" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E189" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="D190" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E190" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D191" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E191" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D192" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E192" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="D193" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E193" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E194" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D195" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E195" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="D197" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D198" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D199" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D200" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E200" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="D201" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D202" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="D203" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="D204" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="D205" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E205" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E206" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="D207" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D208" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E208" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="D209" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E209" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D210" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E210" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="D211" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E211" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="D212" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E212" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D213" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E213" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="D214" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E214" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="E215" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="E216" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="E217" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="E218" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed tabs of dn80 bacterial go terms
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/DN/TD+ND/DN80_combined_TD+ND_bp_GO.xlsx
+++ b/analyses/unipept/GO-terms/DN/TD+ND/DN80_combined_TD+ND_bp_GO.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="DN80_combined_TD+ND_bp_GO" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="revigo" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="organizing" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="for python" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Raw GO counts DN80_combined_TD+" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Revigo condensation" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Manual condensation after Revig" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="condensed for Fig. 6b python sc" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="GO terms &gt;1 peptides" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="1128">
   <si>
     <t xml:space="preserve">GO term</t>
   </si>
@@ -3387,6 +3387,18 @@
   </si>
   <si>
     <t xml:space="preserve">TOO BROAD FOR USE, NOT IN TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0 Bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 2 Bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 5 Bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 12 Bacteria</t>
   </si>
   <si>
     <t xml:space="preserve">Inorganic molecule metabolism</t>
@@ -24386,8 +24398,8 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24400,16 +24412,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>1121</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>1122</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>1123</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24516,7 +24528,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1121</v>
+        <v>1125</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.993377483443709</v>
@@ -24567,7 +24579,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1122</v>
+        <v>1126</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>11.2582781456954</v>
@@ -24584,7 +24596,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1123</v>
+        <v>1127</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>6.62251655629139</v>
@@ -24780,7 +24792,7 @@
   </sheetPr>
   <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C226" activeCellId="0" sqref="C226"/>
     </sheetView>
   </sheetViews>

</xml_diff>